<commit_message>
Verificação do que Está Feito
</commit_message>
<xml_diff>
--- a/Planeamento de Testes.xlsx
+++ b/Planeamento de Testes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\3Ano\BasedeDados2\Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\3Ano\BasedeDados2\Projeto\BD-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B23828-9C14-4B80-920C-E58B887D68B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CD52AE-89EE-4DA3-A211-2A8C0FFD1B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{20B2B5A1-D09A-4E44-B02E-F87ED06015E3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="61">
   <si>
     <t>Teste</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Associar Jogador a uma Posição</t>
   </si>
   <si>
-    <t>Associar Jogador a uma Equipa</t>
-  </si>
-  <si>
     <t>//JOGOS</t>
   </si>
   <si>
@@ -186,6 +183,42 @@
   </si>
   <si>
     <t>Apagar Associação</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Adicionar Vencedor</t>
+  </si>
+  <si>
+    <t>Associar Jogador a um Clube</t>
+  </si>
+  <si>
+    <t>Associar Jogador a uma Equipa do respetivo Clube</t>
+  </si>
+  <si>
+    <t>//UTILIZADORES</t>
+  </si>
+  <si>
+    <t>Criar Conta</t>
+  </si>
+  <si>
+    <t>Conta Admin Criada tem de ser Ativada</t>
+  </si>
+  <si>
+    <t>Terminar Sessão</t>
+  </si>
+  <si>
+    <t>Iniciar Sessão</t>
+  </si>
+  <si>
+    <t>Utilizador tem Clubes Favoritos</t>
+  </si>
+  <si>
+    <t>Associar Clube Vencedor</t>
   </si>
 </sst>
 </file>
@@ -582,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460F8A36-62A1-4866-8461-0429E4ED4873}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,235 +643,475 @@
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>46</v>
       </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>44</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="B17" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="B21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="B25" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="B31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="B35" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="C36" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="B37" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="B38" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="B39" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="B40" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="B43" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
+      <c r="B44" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="B45" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
+      <c r="B46" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="B47" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
+      <c r="B48" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="B49" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
+      <c r="B50" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>42</v>
+      <c r="B51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Planeamento de Testes.xlsx
</commit_message>
<xml_diff>
--- a/Planeamento de Testes.xlsx
+++ b/Planeamento de Testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\3Ano\BasedeDados2\Projeto\BD-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CD52AE-89EE-4DA3-A211-2A8C0FFD1B0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA04EA8-ACC4-4ED4-9E44-B52A5300C912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{20B2B5A1-D09A-4E44-B02E-F87ED06015E3}"/>
   </bookViews>
@@ -267,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -280,6 +280,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460F8A36-62A1-4866-8461-0429E4ED4873}">
   <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -686,9 +689,10 @@
       <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -936,7 +940,7 @@
       <c r="A36" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>50</v>
       </c>
     </row>
@@ -984,7 +988,7 @@
       <c r="A42" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>